<commit_message>
LT working on Manuscript writting and sorting data spreadsheets
</commit_message>
<xml_diff>
--- a/Lloyds_pcrit data.xlsx
+++ b/Lloyds_pcrit data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lloydatrueblood/Desktop/Muusoctopus_leioderma_respiration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0E688C-B228-D84A-9A01-740CB8DC5ED5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4214ED-3539-544D-8FAA-F810095691B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31420" yWindow="2320" windowWidth="27640" windowHeight="16940" activeTab="3" xr2:uid="{1521405B-CA69-7F46-9F39-5092125DF956}"/>
+    <workbookView xWindow="-34880" yWindow="-320" windowWidth="27640" windowHeight="16940" activeTab="3" xr2:uid="{1521405B-CA69-7F46-9F39-5092125DF956}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="81">
   <si>
     <t>Alpha</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>A40</t>
+  </si>
+  <si>
+    <t>After Binned method</t>
   </si>
 </sst>
 </file>
@@ -2937,10 +2940,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10EEA680-4305-E54C-A8A1-00C2C16166D9}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3419,7 +3422,7 @@
         <v>10.365853658536594</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C17">
         <f t="shared" ref="C17:F17" si="13">C11-B11</f>
         <v>311.11111111111114</v>
@@ -3437,7 +3440,7 @@
         <v>250.00000000000011</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C18">
         <f t="shared" ref="C18:F18" si="14">C12-B12</f>
         <v>123.45679012345676</v>
@@ -3453,6 +3456,156 @@
       <c r="F18">
         <f t="shared" si="14"/>
         <v>45.679012345678927</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>0.72</v>
+      </c>
+      <c r="C21">
+        <v>0.91</v>
+      </c>
+      <c r="D21">
+        <v>1.38</v>
+      </c>
+      <c r="E21">
+        <v>1.83</v>
+      </c>
+      <c r="F21">
+        <v>2.16</v>
+      </c>
+      <c r="H21">
+        <v>5</v>
+      </c>
+      <c r="I21">
+        <v>5</v>
+      </c>
+      <c r="J21">
+        <v>5.01</v>
+      </c>
+      <c r="K21">
+        <v>5.09</v>
+      </c>
+      <c r="L21">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22">
+        <v>0.8</v>
+      </c>
+      <c r="C22">
+        <v>1.03</v>
+      </c>
+      <c r="D22">
+        <v>1.44</v>
+      </c>
+      <c r="E22">
+        <v>1.79</v>
+      </c>
+      <c r="F22">
+        <v>1.87</v>
+      </c>
+      <c r="H22">
+        <v>2.6</v>
+      </c>
+      <c r="I22">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="J22">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="K22">
+        <v>2.35</v>
+      </c>
+      <c r="L22">
+        <v>2.34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24">
+        <v>-0.81</v>
+      </c>
+      <c r="C24">
+        <v>1.26</v>
+      </c>
+      <c r="D24">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="E24">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="F24">
+        <v>2.89</v>
+      </c>
+      <c r="H24">
+        <v>18.5</v>
+      </c>
+      <c r="I24">
+        <v>18.5</v>
+      </c>
+      <c r="J24">
+        <v>3.83</v>
+      </c>
+      <c r="K24">
+        <v>3.86</v>
+      </c>
+      <c r="L24">
+        <v>3.83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25">
+        <v>2.38</v>
+      </c>
+      <c r="C25">
+        <v>2.94</v>
+      </c>
+      <c r="D25">
+        <v>3.96</v>
+      </c>
+      <c r="E25">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="F25">
+        <v>4.43</v>
+      </c>
+      <c r="H25">
+        <v>9.5</v>
+      </c>
+      <c r="I25">
+        <v>8.9</v>
+      </c>
+      <c r="J25">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="K25">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="L25">
+        <v>8.8000000000000007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lloyd and Kirt tinkering and sorting data as well as manuscript edits.
</commit_message>
<xml_diff>
--- a/Lloyds_pcrit data.xlsx
+++ b/Lloyds_pcrit data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lloydatrueblood/Desktop/Muusoctopus_leioderma_respiration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lloydatrueblood/Desktop/Desktop files/Muusoctopus_leioderma_respiration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4214ED-3539-544D-8FAA-F810095691B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28719B6-934F-DA4E-8C68-BAAEDB25F4EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34880" yWindow="-320" windowWidth="27640" windowHeight="16940" activeTab="3" xr2:uid="{1521405B-CA69-7F46-9F39-5092125DF956}"/>
+    <workbookView xWindow="40" yWindow="500" windowWidth="17660" windowHeight="20520" xr2:uid="{1521405B-CA69-7F46-9F39-5092125DF956}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -653,7 +653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A34C348-3EE1-3047-9D84-B8D0EFEC49AD}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A35" sqref="A35:XFD38"/>
     </sheetView>
   </sheetViews>
@@ -1638,8 +1638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACABD633-DB3E-B14F-A860-318CF480E83D}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2320,9 +2320,7 @@
       <c r="B25" s="2">
         <v>3</v>
       </c>
-      <c r="C25" s="2">
-        <v>2.39</v>
-      </c>
+      <c r="C25" s="2"/>
       <c r="D25" s="2">
         <v>4.46</v>
       </c>
@@ -2942,7 +2940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10EEA680-4305-E54C-A8A1-00C2C16166D9}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>

</xml_diff>